<commit_message>
Updated the test cases sheet as per the test case identified during test plan review
SVN-Revision: 25479
</commit_message>
<xml_diff>
--- a/TestCases/ToBeAutomated/CollectionProtocol.xlsx
+++ b/TestCases/ToBeAutomated/CollectionProtocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="70">
   <si>
     <t>TestCase</t>
   </si>
@@ -190,6 +190,42 @@
   </si>
   <si>
     <t>CP_Edit_SIteAdmin</t>
+  </si>
+  <si>
+    <t>Share_ CP_ Across_ Sites</t>
+  </si>
+  <si>
+    <t>Edit_Success_CP_Privileges</t>
+  </si>
+  <si>
+    <t>Error_CP_Edit_Privileges</t>
+  </si>
+  <si>
+    <t>Site_ administrator_ share _ CP_  across_ sites</t>
+  </si>
+  <si>
+    <t>Allow/Disallow view data on CP for scientists</t>
+  </si>
+  <si>
+    <t>Site_specific_privilege_CP_level</t>
+  </si>
+  <si>
+    <t>Assign privileges across sites for same protoco</t>
+  </si>
+  <si>
+    <t>Edit_CP_Site_Admin</t>
+  </si>
+  <si>
+    <t>CP_Add_Success</t>
+  </si>
+  <si>
+    <t>CP_Edit_Success</t>
+  </si>
+  <si>
+    <t>CP_Add_error</t>
+  </si>
+  <si>
+    <t>As user w/o privileges</t>
   </si>
 </sst>
 </file>
@@ -543,16 +579,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H50"/>
+  <dimension ref="A2:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="47.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="1" customWidth="1"/>
@@ -665,7 +701,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="60">
+    <row r="11" spans="1:8" ht="45">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
@@ -674,7 +710,7 @@
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="60">
+    <row r="12" spans="1:8" ht="45">
       <c r="A12" s="6" t="s">
         <v>13</v>
       </c>
@@ -683,7 +719,7 @@
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="120">
+    <row r="13" spans="1:8" ht="75">
       <c r="A13" s="6" t="s">
         <v>13</v>
       </c>
@@ -692,7 +728,7 @@
       </c>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:8" ht="90">
+    <row r="14" spans="1:8" ht="60">
       <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
@@ -715,7 +751,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" ht="60">
+    <row r="16" spans="1:8" ht="45">
       <c r="A16" s="6" t="s">
         <v>13</v>
       </c>
@@ -729,7 +765,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" ht="60">
+    <row r="17" spans="1:8" ht="45">
       <c r="A17" s="6" t="s">
         <v>22</v>
       </c>
@@ -757,7 +793,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" ht="60">
+    <row r="19" spans="1:8" ht="45">
       <c r="A19" s="6" t="s">
         <v>22</v>
       </c>
@@ -771,7 +807,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" ht="60">
+    <row r="20" spans="1:8" ht="45">
       <c r="A20" s="6" t="s">
         <v>22</v>
       </c>
@@ -785,7 +821,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="120">
+    <row r="21" spans="1:8" ht="75">
       <c r="A21" s="6" t="s">
         <v>22</v>
       </c>
@@ -799,7 +835,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="90">
+    <row r="22" spans="1:8" ht="60">
       <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
@@ -827,7 +863,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" ht="60">
+    <row r="24" spans="1:8" ht="45">
       <c r="A24" s="6" t="s">
         <v>22</v>
       </c>
@@ -929,7 +965,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="45">
+    <row r="29" spans="1:8" ht="30">
       <c r="A29" s="6" t="s">
         <v>38</v>
       </c>
@@ -955,7 +991,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="45">
+    <row r="30" spans="1:8" ht="30">
       <c r="A30" s="6" t="s">
         <v>43</v>
       </c>
@@ -981,7 +1017,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="45">
+    <row r="31" spans="1:8">
       <c r="A31" s="6" t="s">
         <v>47</v>
       </c>
@@ -1007,7 +1043,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="60">
+    <row r="32" spans="1:8" ht="45">
       <c r="A32" s="6" t="s">
         <v>49</v>
       </c>
@@ -1021,7 +1057,7 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" ht="105">
+    <row r="33" spans="1:8" ht="60">
       <c r="A33" s="6" t="s">
         <v>49</v>
       </c>
@@ -1035,7 +1071,7 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8" ht="45">
+    <row r="34" spans="1:8" ht="30">
       <c r="A34" s="6" t="s">
         <v>49</v>
       </c>
@@ -1049,7 +1085,7 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" ht="45">
+    <row r="35" spans="1:8">
       <c r="A35" s="6" t="s">
         <v>49</v>
       </c>
@@ -1065,7 +1101,7 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" ht="45">
+    <row r="36" spans="1:8">
       <c r="A36" s="6" t="s">
         <v>49</v>
       </c>
@@ -1079,7 +1115,7 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8" ht="45">
+    <row r="37" spans="1:8" ht="30">
       <c r="A37" s="6" t="s">
         <v>49</v>
       </c>
@@ -1095,7 +1131,7 @@
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="1:8" ht="45">
+    <row r="38" spans="1:8" ht="30">
       <c r="A38" s="6" t="s">
         <v>49</v>
       </c>
@@ -1111,7 +1147,7 @@
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:8" ht="45">
+    <row r="39" spans="1:8">
       <c r="A39" s="6" t="s">
         <v>49</v>
       </c>
@@ -1125,7 +1161,7 @@
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" spans="1:8" ht="45">
+    <row r="40" spans="1:8">
       <c r="A40" s="6" t="s">
         <v>53</v>
       </c>
@@ -1137,7 +1173,7 @@
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" spans="1:8" ht="45">
+    <row r="41" spans="1:8">
       <c r="A41" s="6" t="s">
         <v>54</v>
       </c>
@@ -1151,7 +1187,7 @@
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
     </row>
-    <row r="42" spans="1:8" ht="45">
+    <row r="42" spans="1:8" ht="30">
       <c r="A42" s="6" t="s">
         <v>54</v>
       </c>
@@ -1165,7 +1201,7 @@
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
     </row>
-    <row r="43" spans="1:8" ht="60">
+    <row r="43" spans="1:8" ht="45">
       <c r="A43" s="6" t="s">
         <v>57</v>
       </c>
@@ -1193,7 +1229,7 @@
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
     </row>
-    <row r="45" spans="1:8" ht="60">
+    <row r="45" spans="1:8" ht="45">
       <c r="A45" s="6" t="s">
         <v>57</v>
       </c>
@@ -1207,7 +1243,7 @@
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
     </row>
-    <row r="46" spans="1:8" ht="60">
+    <row r="46" spans="1:8" ht="45">
       <c r="A46" s="6" t="s">
         <v>57</v>
       </c>
@@ -1221,7 +1257,7 @@
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
     </row>
-    <row r="47" spans="1:8" ht="120">
+    <row r="47" spans="1:8" ht="75">
       <c r="A47" s="6" t="s">
         <v>57</v>
       </c>
@@ -1229,7 +1265,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="90">
+    <row r="48" spans="1:8" ht="60">
       <c r="A48" s="6" t="s">
         <v>57</v>
       </c>
@@ -1245,12 +1281,84 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="60">
+    <row r="50" spans="1:2" ht="45">
       <c r="A50" s="6" t="s">
         <v>57</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>